<commit_message>
prototype of tree and operational symbols.
</commit_message>
<xml_diff>
--- a/backend/cpp-custom/internal/ll1/specifications/LL_table.xlsx
+++ b/backend/cpp-custom/internal/ll1/specifications/LL_table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="113">
   <si>
     <t>EPSILON</t>
   </si>
@@ -111,9 +111,6 @@
     <t>PD</t>
   </si>
   <si>
-    <t>PD1 void</t>
-  </si>
-  <si>
     <t>PD1</t>
   </si>
   <si>
@@ -129,12 +126,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>; VS</t>
-  </si>
-  <si>
-    <t>; CS</t>
-  </si>
-  <si>
     <t>VS</t>
   </si>
   <si>
@@ -192,9 +183,6 @@
     <t>CO</t>
   </si>
   <si>
-    <t>} OD {</t>
-  </si>
-  <si>
     <t>OD</t>
   </si>
   <si>
@@ -231,9 +219,6 @@
     <t>PS ,</t>
   </si>
   <si>
-    <t>O ) FA ; FE ; OF1 ( for</t>
-  </si>
-  <si>
     <t>OF1</t>
   </si>
   <si>
@@ -327,21 +312,6 @@
     <t>CONSTANT</t>
   </si>
   <si>
-    <t>CO ) PSD ( IDENTITY</t>
-  </si>
-  <si>
-    <t>PSD1 IDENTITY T</t>
-  </si>
-  <si>
-    <t>FV1 IDENTITY T</t>
-  </si>
-  <si>
-    <t>V1 IDENTITY</t>
-  </si>
-  <si>
-    <t>E = IDENTITY T const</t>
-  </si>
-  <si>
     <t>E = IDENTITY</t>
   </si>
   <si>
@@ -354,7 +324,40 @@
     <t>PS1 CONSTANT</t>
   </si>
   <si>
-    <t>E = IDENTITY T</t>
+    <t>CO ) PSD ( #pi IDENTITY</t>
+  </si>
+  <si>
+    <t>PSD1 #pad IDENTITY T</t>
+  </si>
+  <si>
+    <t>#epd PD1 #spd void</t>
+  </si>
+  <si>
+    <t>} #eco OD #sco {</t>
+  </si>
+  <si>
+    <t>; #evd VS #svd</t>
+  </si>
+  <si>
+    <t>FV1 #fvd IDENTITY T</t>
+  </si>
+  <si>
+    <t>V1 #vd IDENTITY</t>
+  </si>
+  <si>
+    <t>; #encd CS #sncd</t>
+  </si>
+  <si>
+    <t>E = #fncd IDENTITY T const</t>
+  </si>
+  <si>
+    <t>E = #ncd IDENTITY</t>
+  </si>
+  <si>
+    <t>#efl O ) FA ; FE ; OF1 ( for #sfl</t>
+  </si>
+  <si>
+    <t>E = #flcd IDENTITY T</t>
   </si>
 </sst>
 </file>
@@ -758,40 +761,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG367"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z32" sqref="Z32"/>
+      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="21.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="12" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.88671875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.21875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.109375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.5546875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="10.21875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="11.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.77734375" style="1" customWidth="1"/>
+    <col min="6" max="9" width="26.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.77734375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.21875" style="1" customWidth="1"/>
+    <col min="15" max="16" width="10.77734375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="4.5546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.77734375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11.5546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="11.109375" style="1" customWidth="1"/>
+    <col min="24" max="25" width="11.5546875" style="1" customWidth="1"/>
+    <col min="26" max="27" width="10.77734375" style="1" customWidth="1"/>
+    <col min="28" max="28" width="10.21875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="10" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.88671875" style="1" customWidth="1"/>
     <col min="31" max="32" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -801,10 +803,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -896,49 +898,49 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B3" s="3"/>
       <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>7</v>
@@ -949,32 +951,32 @@
         <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>0</v>
@@ -982,83 +984,83 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>0</v>
@@ -1067,20 +1069,20 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>0</v>
@@ -1089,56 +1091,56 @@
         <v>0</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>8</v>
@@ -1146,45 +1148,45 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>0</v>
@@ -1192,44 +1194,44 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>0</v>
@@ -1237,52 +1239,52 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>0</v>
@@ -1290,33 +1292,33 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>0</v>
@@ -1324,27 +1326,27 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="M32" s="1" t="s">
         <v>0</v>
@@ -1356,41 +1358,41 @@
         <v>0</v>
       </c>
       <c r="V32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="X32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA32" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="W32" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="X32" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y32" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA32" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>0</v>
@@ -1402,10 +1404,10 @@
         <v>0</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>0</v>
@@ -1428,71 +1430,71 @@
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA36" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB36" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC36" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="AD36" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A37" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
sem. tree and operational symbols.
</commit_message>
<xml_diff>
--- a/backend/cpp-custom/internal/ll1/specifications/LL_table.xlsx
+++ b/backend/cpp-custom/internal/ll1/specifications/LL_table.xlsx
@@ -330,24 +330,15 @@
     <t>PSD1 #pad IDENTITY T</t>
   </si>
   <si>
-    <t>#epd PD1 #spd void</t>
-  </si>
-  <si>
     <t>} #eco OD #sco {</t>
   </si>
   <si>
-    <t>; #evd VS #svd</t>
-  </si>
-  <si>
     <t>FV1 #fvd IDENTITY T</t>
   </si>
   <si>
     <t>V1 #vd IDENTITY</t>
   </si>
   <si>
-    <t>; #encd CS #sncd</t>
-  </si>
-  <si>
     <t>E = #fncd IDENTITY T const</t>
   </si>
   <si>
@@ -358,6 +349,15 @@
   </si>
   <si>
     <t>E = #flcd IDENTITY T</t>
+  </si>
+  <si>
+    <t>#epd PD1 void</t>
+  </si>
+  <si>
+    <t>; #evd VS</t>
+  </si>
+  <si>
+    <t>; #encd CS</t>
   </si>
 </sst>
 </file>
@@ -762,10 +762,10 @@
   <dimension ref="A1:AG367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.4"/>
@@ -951,7 +951,7 @@
         <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.4">
@@ -998,19 +998,19 @@
         <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.4">
@@ -1046,16 +1046,16 @@
         <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.4">
@@ -1077,7 +1077,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.4">
@@ -1118,7 +1118,7 @@
         <v>48</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.4">
@@ -1126,7 +1126,7 @@
         <v>49</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.4">
@@ -1151,7 +1151,7 @@
         <v>53</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.4">
@@ -1264,7 +1264,7 @@
         <v>58</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.4">
@@ -1275,16 +1275,16 @@
         <v>97</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M28" s="1" t="s">
         <v>0</v>

</xml_diff>